<commit_message>
Add hostid in table
</commit_message>
<xml_diff>
--- a/table-template.xlsx
+++ b/table-template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Hostname</t>
   </si>
@@ -28,6 +28,9 @@
     <t>IP address</t>
   </si>
   <si>
+    <t>DNS</t>
+  </si>
+  <si>
     <t>Port</t>
   </si>
   <si>
@@ -58,16 +61,22 @@
     <t>Serial number</t>
   </si>
   <si>
+    <t>hostid</t>
+  </si>
+  <si>
     <t>TEST1</t>
   </si>
   <si>
     <t>Zabbix servers, test</t>
   </si>
   <si>
+    <t>Disabled</t>
+  </si>
+  <si>
     <t>10.10.14.1</t>
   </si>
   <si>
-    <t>1</t>
+    <t>Agent</t>
   </si>
   <si>
     <t xml:space="preserve">ICMP Ping, Linux by Zabbix agent
@@ -139,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -147,6 +156,9 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -159,7 +171,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -464,26 +482,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="34.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="16.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="34.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="6" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="8" width="13.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -499,13 +519,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -520,59 +540,67 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="5">
         <v>10500</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2">
         <v>123456</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>